<commit_message>
re-organize graphics and resources
</commit_message>
<xml_diff>
--- a/resources/Methodology_Matrix.xlsx
+++ b/resources/Methodology_Matrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Google Drive\Academics\Projects\2020\Complete Streets Bike LOS\Prototype\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Google Drive\Academics\Projects\2020\Complete Streets Bike LOS\Prototype\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB5DA98-07AF-49A4-82A3-A44615E4F035}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361B710E-DCD1-4B78-8A2C-651313E8EDBB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29070" yWindow="930" windowWidth="24360" windowHeight="13590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="150" windowWidth="27930" windowHeight="15180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="92">
   <si>
     <t>Mode</t>
   </si>
@@ -572,7 +572,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -683,6 +683,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -940,8 +941,8 @@
   <dimension ref="A1:AB1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K33" sqref="K33"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1667,7 +1668,9 @@
       <c r="J27" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="K27" s="19"/>
+      <c r="K27" s="58" t="s">
+        <v>13</v>
+      </c>
       <c r="L27" s="20" t="s">
         <v>54</v>
       </c>

</xml_diff>